<commit_message>
charting script mostly done
</commit_message>
<xml_diff>
--- a/film charting stafford 2016.xlsx
+++ b/film charting stafford 2016.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpw/Desktop/andy_benoit_charting_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="12220"/>
   </bookViews>
   <sheets>
     <sheet name="Drive Chart" sheetId="1" r:id="rId1"/>
@@ -151,9 +151,15 @@
     <definedName name="pbp_97" localSheetId="0">'Drive Chart'!#REF!</definedName>
     <definedName name="pbp_99" localSheetId="0">'Drive Chart'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -2107,7 +2113,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2643,36 +2649,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ305"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J306" sqref="J306"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="8.85546875" style="8"/>
-    <col min="3" max="4" width="8.85546875" style="2"/>
-    <col min="5" max="5" width="9.7109375" style="8" customWidth="1"/>
-    <col min="6" max="7" width="8.85546875" style="8"/>
-    <col min="8" max="8" width="8.85546875" style="2"/>
-    <col min="9" max="9" width="13.85546875" style="8" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" style="8"/>
+    <col min="3" max="4" width="8.83203125" style="2"/>
+    <col min="5" max="5" width="9.6640625" style="8" customWidth="1"/>
+    <col min="6" max="7" width="8.83203125" style="8"/>
+    <col min="8" max="8" width="8.83203125" style="2"/>
+    <col min="9" max="9" width="13.83203125" style="8" customWidth="1"/>
     <col min="10" max="10" width="10" style="8" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="16.1640625" style="8" customWidth="1"/>
     <col min="12" max="12" width="12" style="8" customWidth="1"/>
-    <col min="13" max="14" width="8.85546875" style="8"/>
-    <col min="15" max="15" width="13.85546875" style="8" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" style="8" bestFit="1" customWidth="1"/>
-    <col min="17" max="22" width="8.85546875" style="8"/>
-    <col min="23" max="23" width="8.85546875" style="2"/>
-    <col min="24" max="26" width="8.85546875" style="8"/>
-    <col min="27" max="27" width="12.140625" style="8" customWidth="1"/>
-    <col min="28" max="16384" width="8.85546875" style="8"/>
+    <col min="13" max="14" width="8.83203125" style="8"/>
+    <col min="15" max="15" width="13.83203125" style="8" customWidth="1"/>
+    <col min="16" max="16" width="12.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="22" width="8.83203125" style="8"/>
+    <col min="23" max="23" width="8.83203125" style="2"/>
+    <col min="24" max="26" width="8.83203125" style="8"/>
+    <col min="27" max="27" width="12.1640625" style="8" customWidth="1"/>
+    <col min="28" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="1"/>
@@ -2712,7 +2718,7 @@
       <c r="AI1" s="6"/>
       <c r="AJ1" s="7"/>
     </row>
-    <row r="2" spans="1:36" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -2818,7 +2824,7 @@
       </c>
       <c r="AJ2" s="16"/>
     </row>
-    <row r="3" spans="1:36" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -2888,7 +2894,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:36" ht="57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" ht="42" x14ac:dyDescent="0.15">
       <c r="A4" s="18">
         <v>1</v>
       </c>
@@ -2965,7 +2971,7 @@
       <c r="AI4" s="17"/>
       <c r="AJ4" s="17"/>
     </row>
-    <row r="5" spans="1:36" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="18">
         <v>1</v>
       </c>
@@ -3031,7 +3037,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="18">
         <v>1</v>
       </c>
@@ -3098,7 +3104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:36" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" ht="28" x14ac:dyDescent="0.15">
       <c r="A7" s="18">
         <v>1</v>
       </c>
@@ -3161,7 +3167,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:36" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" ht="28" x14ac:dyDescent="0.15">
       <c r="A8" s="18">
         <v>1</v>
       </c>
@@ -3226,7 +3232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="57" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" ht="42" x14ac:dyDescent="0.15">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -3291,7 +3297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:36" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" ht="28" x14ac:dyDescent="0.15">
       <c r="A10" s="18">
         <v>1</v>
       </c>
@@ -3354,7 +3360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" ht="28" x14ac:dyDescent="0.15">
       <c r="A11" s="18">
         <v>1</v>
       </c>
@@ -3419,7 +3425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:36" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" ht="28" x14ac:dyDescent="0.15">
       <c r="A12" s="18">
         <v>1</v>
       </c>
@@ -3482,7 +3488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" ht="28" x14ac:dyDescent="0.15">
       <c r="A13" s="18">
         <v>1</v>
       </c>
@@ -3545,7 +3551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" ht="28" x14ac:dyDescent="0.15">
       <c r="A14" s="18">
         <v>1</v>
       </c>
@@ -3610,7 +3616,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:36" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" ht="28" x14ac:dyDescent="0.15">
       <c r="A15" s="18">
         <v>1</v>
       </c>
@@ -3669,7 +3675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" ht="28" x14ac:dyDescent="0.15">
       <c r="A16" s="18">
         <v>1</v>
       </c>
@@ -3734,7 +3740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A17" s="18">
         <v>1</v>
       </c>
@@ -3797,7 +3803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A18" s="18">
         <v>1</v>
       </c>
@@ -3860,7 +3866,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A19" s="18">
         <v>1</v>
       </c>
@@ -3927,7 +3933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A20" s="18">
         <v>1</v>
       </c>
@@ -3990,7 +3996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A21" s="18">
         <v>1</v>
       </c>
@@ -4053,7 +4059,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A22" s="18">
         <v>1</v>
       </c>
@@ -4116,7 +4122,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A23" s="18">
         <v>1</v>
       </c>
@@ -4179,7 +4185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A24" s="18">
         <v>1</v>
       </c>
@@ -4242,7 +4248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A25" s="18">
         <v>1</v>
       </c>
@@ -4305,7 +4311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A26" s="18">
         <v>1</v>
       </c>
@@ -4362,7 +4368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="56" x14ac:dyDescent="0.15">
       <c r="A27" s="18">
         <v>1</v>
       </c>
@@ -4427,7 +4433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A28" s="18">
         <v>1</v>
       </c>
@@ -4490,7 +4496,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A29" s="18">
         <v>1</v>
       </c>
@@ -4553,7 +4559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A30" s="18">
         <v>1</v>
       </c>
@@ -4616,7 +4622,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A31" s="18">
         <v>1</v>
       </c>
@@ -4679,7 +4685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A32" s="18">
         <v>1</v>
       </c>
@@ -4742,7 +4748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A33" s="18">
         <v>1</v>
       </c>
@@ -4805,7 +4811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A34" s="18">
         <v>1</v>
       </c>
@@ -4868,7 +4874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A35" s="18">
         <v>1</v>
       </c>
@@ -4931,7 +4937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="57" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" ht="56" x14ac:dyDescent="0.15">
       <c r="A36" s="18">
         <v>1</v>
       </c>
@@ -4994,7 +5000,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A37" s="18">
         <v>1</v>
       </c>
@@ -5059,7 +5065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A38" s="18">
         <v>1</v>
       </c>
@@ -5122,7 +5128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A39" s="18">
         <v>1</v>
       </c>
@@ -5185,7 +5191,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A40" s="18">
         <v>1</v>
       </c>
@@ -5248,7 +5254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" s="18">
         <v>1</v>
       </c>
@@ -5311,7 +5317,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A42" s="18">
         <v>1</v>
       </c>
@@ -5374,7 +5380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A43" s="18">
         <v>1</v>
       </c>
@@ -5433,7 +5439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A44" s="8">
         <v>2</v>
       </c>
@@ -5489,7 +5495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A45" s="8">
         <v>2</v>
       </c>
@@ -5548,7 +5554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A46" s="8">
         <v>2</v>
       </c>
@@ -5604,7 +5610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A47" s="8">
         <v>2</v>
       </c>
@@ -5660,7 +5666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A48" s="8">
         <v>2</v>
       </c>
@@ -5716,7 +5722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A49" s="8">
         <v>2</v>
       </c>
@@ -5772,7 +5778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A50" s="8">
         <v>2</v>
       </c>
@@ -5828,7 +5834,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:25" ht="57" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" ht="42" x14ac:dyDescent="0.15">
       <c r="A51" s="8">
         <v>2</v>
       </c>
@@ -5887,7 +5893,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A52" s="8">
         <v>2</v>
       </c>
@@ -5946,7 +5952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A53" s="8">
         <v>2</v>
       </c>
@@ -6002,7 +6008,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A54" s="8">
         <v>2</v>
       </c>
@@ -6058,7 +6064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A55" s="8">
         <v>2</v>
       </c>
@@ -6114,7 +6120,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:25" ht="57" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" ht="42" x14ac:dyDescent="0.15">
       <c r="A56" s="8">
         <v>2</v>
       </c>
@@ -6173,7 +6179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A57" s="8">
         <v>2</v>
       </c>
@@ -6229,7 +6235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A58" s="8">
         <v>2</v>
       </c>
@@ -6291,7 +6297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A59" s="8">
         <v>2</v>
       </c>
@@ -6350,7 +6356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:25" ht="57" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" ht="56" x14ac:dyDescent="0.15">
       <c r="A60" s="8">
         <v>2</v>
       </c>
@@ -6409,7 +6415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A61" s="8">
         <v>2</v>
       </c>
@@ -6465,7 +6471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A62" s="8">
         <v>2</v>
       </c>
@@ -6515,7 +6521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A63" s="8">
         <v>2</v>
       </c>
@@ -6562,7 +6568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A64" s="8">
         <v>2</v>
       </c>
@@ -6618,7 +6624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A65" s="8">
         <v>2</v>
       </c>
@@ -6665,7 +6671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A66" s="8">
         <v>2</v>
       </c>
@@ -6724,7 +6730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A67" s="8">
         <v>2</v>
       </c>
@@ -6786,7 +6792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:25" ht="84" x14ac:dyDescent="0.15">
       <c r="A68" s="8">
         <v>2</v>
       </c>
@@ -6848,7 +6854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A69" s="8">
         <v>2</v>
       </c>
@@ -6904,7 +6910,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A70" s="8">
         <v>2</v>
       </c>
@@ -6960,7 +6966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A71" s="8">
         <v>2</v>
       </c>
@@ -7022,7 +7028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A72" s="8">
         <v>2</v>
       </c>
@@ -7078,7 +7084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A73" s="8">
         <v>2</v>
       </c>
@@ -7134,7 +7140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A74" s="8">
         <v>2</v>
       </c>
@@ -7193,7 +7199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A75" s="8">
         <v>2</v>
       </c>
@@ -7249,7 +7255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A76" s="8">
         <v>2</v>
       </c>
@@ -7308,7 +7314,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A77" s="8">
         <v>2</v>
       </c>
@@ -7358,7 +7364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A78" s="8">
         <v>2</v>
       </c>
@@ -7414,7 +7420,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A79" s="8">
         <v>2</v>
       </c>
@@ -7470,7 +7476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A80" s="8">
         <v>2</v>
       </c>
@@ -7526,7 +7532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A81" s="8">
         <v>2</v>
       </c>
@@ -7582,7 +7588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A82" s="8">
         <v>2</v>
       </c>
@@ -7638,7 +7644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A83" s="8">
         <v>2</v>
       </c>
@@ -7685,7 +7691,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A84" s="8">
         <v>2</v>
       </c>
@@ -7741,7 +7747,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A85" s="8">
         <v>2</v>
       </c>
@@ -7797,7 +7803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A86" s="8">
         <v>2</v>
       </c>
@@ -7853,7 +7859,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A87" s="8">
         <v>2</v>
       </c>
@@ -7912,7 +7918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A88" s="8">
         <v>3</v>
       </c>
@@ -7962,7 +7968,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A89" s="8">
         <v>3</v>
       </c>
@@ -8018,7 +8024,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A90" s="8">
         <v>3</v>
       </c>
@@ -8074,7 +8080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A91" s="8">
         <v>3</v>
       </c>
@@ -8133,7 +8139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A92" s="8">
         <v>3</v>
       </c>
@@ -8189,7 +8195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A93" s="8">
         <v>3</v>
       </c>
@@ -8245,7 +8251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A94" s="8">
         <v>3</v>
       </c>
@@ -8304,7 +8310,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A95" s="8">
         <v>3</v>
       </c>
@@ -8360,7 +8366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A96" s="8">
         <v>3</v>
       </c>
@@ -8419,7 +8425,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A97" s="8">
         <v>3</v>
       </c>
@@ -8478,7 +8484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A98" s="8">
         <v>3</v>
       </c>
@@ -8534,7 +8540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A99" s="8">
         <v>3</v>
       </c>
@@ -8590,7 +8596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A100" s="8">
         <v>3</v>
       </c>
@@ -8643,7 +8649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A101" s="8">
         <v>3</v>
       </c>
@@ -8699,7 +8705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A102" s="8">
         <v>3</v>
       </c>
@@ -8758,7 +8764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A103" s="8">
         <v>3</v>
       </c>
@@ -8817,7 +8823,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A104" s="8">
         <v>3</v>
       </c>
@@ -8873,7 +8879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A105" s="8">
         <v>3</v>
       </c>
@@ -8929,7 +8935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A106" s="8">
         <v>3</v>
       </c>
@@ -8985,7 +8991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A107" s="8">
         <v>3</v>
       </c>
@@ -9041,7 +9047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A108" s="8">
         <v>3</v>
       </c>
@@ -9097,7 +9103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A109" s="8">
         <v>3</v>
       </c>
@@ -9153,7 +9159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A110" s="8">
         <v>3</v>
       </c>
@@ -9209,7 +9215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A111" s="8">
         <v>3</v>
       </c>
@@ -9265,7 +9271,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A112" s="8">
         <v>3</v>
       </c>
@@ -9321,7 +9327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A113" s="8">
         <v>3</v>
       </c>
@@ -9377,7 +9383,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A114" s="8">
         <v>3</v>
       </c>
@@ -9433,7 +9439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A115" s="8">
         <v>3</v>
       </c>
@@ -9492,7 +9498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A116" s="8">
         <v>3</v>
       </c>
@@ -9548,7 +9554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A117" s="8">
         <v>3</v>
       </c>
@@ -9604,7 +9610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A118" s="8">
         <v>3</v>
       </c>
@@ -9660,7 +9666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A119" s="8">
         <v>3</v>
       </c>
@@ -9716,7 +9722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A120" s="8">
         <v>3</v>
       </c>
@@ -9772,7 +9778,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A121" s="8">
         <v>3</v>
       </c>
@@ -9828,7 +9834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A122" s="8">
         <v>3</v>
       </c>
@@ -9875,7 +9881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A123" s="8">
         <v>3</v>
       </c>
@@ -9934,7 +9940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A124" s="8">
         <v>3</v>
       </c>
@@ -9984,7 +9990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A125" s="8">
         <v>3</v>
       </c>
@@ -10040,7 +10046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A126" s="8">
         <v>3</v>
       </c>
@@ -10087,7 +10093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A127" s="8">
         <v>3</v>
       </c>
@@ -10143,7 +10149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A128" s="8">
         <v>3</v>
       </c>
@@ -10199,7 +10205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A129" s="8">
         <v>3</v>
       </c>
@@ -10255,7 +10261,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A130" s="8">
         <v>3</v>
       </c>
@@ -10311,7 +10317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A131" s="8">
         <v>3</v>
       </c>
@@ -10367,7 +10373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A132" s="8">
         <v>4</v>
       </c>
@@ -10423,7 +10429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A133" s="8">
         <v>4</v>
       </c>
@@ -10479,7 +10485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:25" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:25" ht="70" x14ac:dyDescent="0.15">
       <c r="A134" s="8">
         <v>4</v>
       </c>
@@ -10535,7 +10541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A135" s="8">
         <v>4</v>
       </c>
@@ -10591,7 +10597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A136" s="8">
         <v>4</v>
       </c>
@@ -10647,7 +10653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A137" s="8">
         <v>4</v>
       </c>
@@ -10706,7 +10712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A138" s="8">
         <v>4</v>
       </c>
@@ -10753,7 +10759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A139" s="8">
         <v>4</v>
       </c>
@@ -10809,7 +10815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:25" ht="42" x14ac:dyDescent="0.15">
       <c r="A140" s="8">
         <v>4</v>
       </c>
@@ -10871,7 +10877,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A141" s="8">
         <v>4</v>
       </c>
@@ -10927,7 +10933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A142" s="8">
         <v>4</v>
       </c>
@@ -10983,7 +10989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A143" s="8">
         <v>4</v>
       </c>
@@ -11039,7 +11045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A144" s="8">
         <v>4</v>
       </c>
@@ -11098,7 +11104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A145" s="8">
         <v>4</v>
       </c>
@@ -11154,7 +11160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A146" s="8">
         <v>4</v>
       </c>
@@ -11210,7 +11216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A147" s="8">
         <v>4</v>
       </c>
@@ -11269,7 +11275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A148" s="8">
         <v>4</v>
       </c>
@@ -11325,7 +11331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A149" s="8">
         <v>4</v>
       </c>
@@ -11381,7 +11387,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A150" s="8">
         <v>4</v>
       </c>
@@ -11437,7 +11443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A151" s="8">
         <v>4</v>
       </c>
@@ -11493,7 +11499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A152" s="8">
         <v>4</v>
       </c>
@@ -11549,7 +11555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A153" s="8">
         <v>4</v>
       </c>
@@ -11605,7 +11611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A154" s="8">
         <v>4</v>
       </c>
@@ -11664,7 +11670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A155" s="8">
         <v>4</v>
       </c>
@@ -11723,7 +11729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A156" s="8">
         <v>4</v>
       </c>
@@ -11779,7 +11785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A157" s="8">
         <v>4</v>
       </c>
@@ -11835,7 +11841,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A158" s="8">
         <v>4</v>
       </c>
@@ -11894,7 +11900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A159" s="8">
         <v>4</v>
       </c>
@@ -11950,7 +11956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A160" s="8">
         <v>4</v>
       </c>
@@ -12006,7 +12012,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A161" s="8">
         <v>4</v>
       </c>
@@ -12065,7 +12071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A162" s="8">
         <v>4</v>
       </c>
@@ -12121,7 +12127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A163" s="8">
         <v>4</v>
       </c>
@@ -12177,7 +12183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A164" s="8">
         <v>4</v>
       </c>
@@ -12224,7 +12230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A165" s="8">
         <v>4</v>
       </c>
@@ -12280,7 +12286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A166" s="8">
         <v>4</v>
       </c>
@@ -12339,7 +12345,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A167" s="8">
         <v>4</v>
       </c>
@@ -12395,7 +12401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A168" s="8">
         <v>4</v>
       </c>
@@ -12454,7 +12460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A169" s="8">
         <v>4</v>
       </c>
@@ -12513,7 +12519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A170" s="8">
         <v>4</v>
       </c>
@@ -12569,7 +12575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A171" s="8">
         <v>5</v>
       </c>
@@ -12625,7 +12631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A172" s="8">
         <v>5</v>
       </c>
@@ -12681,7 +12687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A173" s="8">
         <v>5</v>
       </c>
@@ -12737,7 +12743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A174" s="8">
         <v>5</v>
       </c>
@@ -12793,7 +12799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A175" s="8">
         <v>5</v>
       </c>
@@ -12849,7 +12855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A176" s="8">
         <v>5</v>
       </c>
@@ -12908,7 +12914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A177" s="8">
         <v>5</v>
       </c>
@@ -12964,7 +12970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A178" s="8">
         <v>5</v>
       </c>
@@ -13020,7 +13026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A179" s="8">
         <v>5</v>
       </c>
@@ -13079,7 +13085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A180" s="8">
         <v>5</v>
       </c>
@@ -13135,7 +13141,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A181" s="8">
         <v>5</v>
       </c>
@@ -13191,7 +13197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A182" s="8">
         <v>5</v>
       </c>
@@ -13250,7 +13256,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A183" s="8">
         <v>5</v>
       </c>
@@ -13300,7 +13306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A184" s="8">
         <v>5</v>
       </c>
@@ -13359,7 +13365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A185" s="8">
         <v>5</v>
       </c>
@@ -13415,7 +13421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:25" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:25" ht="84" x14ac:dyDescent="0.15">
       <c r="A186" s="8">
         <v>5</v>
       </c>
@@ -13468,7 +13474,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:25" ht="42" x14ac:dyDescent="0.15">
       <c r="A187" s="8">
         <v>5</v>
       </c>
@@ -13515,7 +13521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A188" s="8">
         <v>5</v>
       </c>
@@ -13571,7 +13577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A189" s="8">
         <v>5</v>
       </c>
@@ -13627,7 +13633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A190" s="8">
         <v>5</v>
       </c>
@@ -13677,7 +13683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A191" s="8">
         <v>5</v>
       </c>
@@ -13733,7 +13739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A192" s="8">
         <v>5</v>
       </c>
@@ -13789,7 +13795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A193" s="8">
         <v>5</v>
       </c>
@@ -13836,7 +13842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A194" s="8">
         <v>5</v>
       </c>
@@ -13895,7 +13901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A195" s="8">
         <v>5</v>
       </c>
@@ -13951,7 +13957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A196" s="8">
         <v>5</v>
       </c>
@@ -14007,7 +14013,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A197" s="8">
         <v>5</v>
       </c>
@@ -14063,7 +14069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:25" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:25" ht="98" x14ac:dyDescent="0.15">
       <c r="A198" s="8">
         <v>5</v>
       </c>
@@ -14122,7 +14128,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A199" s="8">
         <v>5</v>
       </c>
@@ -14169,7 +14175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A200" s="8">
         <v>6</v>
       </c>
@@ -14228,7 +14234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A201" s="8">
         <v>6</v>
       </c>
@@ -14284,7 +14290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:25" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:25" ht="56" x14ac:dyDescent="0.15">
       <c r="A202" s="8">
         <v>6</v>
       </c>
@@ -14343,7 +14349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A203" s="8">
         <v>6</v>
       </c>
@@ -14399,7 +14405,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A204" s="8">
         <v>6</v>
       </c>
@@ -14455,7 +14461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A205" s="8">
         <v>6</v>
       </c>
@@ -14511,7 +14517,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="206" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A206" s="8">
         <v>6</v>
       </c>
@@ -14570,7 +14576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A207" s="8">
         <v>6</v>
       </c>
@@ -14632,7 +14638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A208" s="8">
         <v>6</v>
       </c>
@@ -14688,7 +14694,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A209" s="8">
         <v>6</v>
       </c>
@@ -14747,7 +14753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A210" s="8">
         <v>6</v>
       </c>
@@ -14806,7 +14812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="211" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A211" s="8">
         <v>6</v>
       </c>
@@ -14862,7 +14868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:25" ht="42" x14ac:dyDescent="0.15">
       <c r="A212" s="8">
         <v>6</v>
       </c>
@@ -14921,7 +14927,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="213" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A213" s="8">
         <v>6</v>
       </c>
@@ -14977,7 +14983,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A214" s="8">
         <v>6</v>
       </c>
@@ -15039,7 +15045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A215" s="8">
         <v>6</v>
       </c>
@@ -15098,7 +15104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="216" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A216" s="8">
         <v>6</v>
       </c>
@@ -15157,7 +15163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A217" s="8">
         <v>6</v>
       </c>
@@ -15216,7 +15222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A218" s="8">
         <v>6</v>
       </c>
@@ -15272,7 +15278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A219" s="8">
         <v>6</v>
       </c>
@@ -15328,7 +15334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:25" ht="42" x14ac:dyDescent="0.15">
       <c r="A220" s="8">
         <v>6</v>
       </c>
@@ -15384,7 +15390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A221" s="8">
         <v>6</v>
       </c>
@@ -15440,7 +15446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A222" s="8">
         <v>6</v>
       </c>
@@ -15496,7 +15502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A223" s="8">
         <v>6</v>
       </c>
@@ -15552,7 +15558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A224" s="8">
         <v>6</v>
       </c>
@@ -15611,7 +15617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A225" s="8">
         <v>6</v>
       </c>
@@ -15667,7 +15673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="226" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A226" s="8">
         <v>6</v>
       </c>
@@ -15723,7 +15729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A227" s="8">
         <v>6</v>
       </c>
@@ -15779,7 +15785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="228" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A228" s="8">
         <v>6</v>
       </c>
@@ -15841,7 +15847,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A229" s="8">
         <v>6</v>
       </c>
@@ -15888,7 +15894,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A230" s="8">
         <v>6</v>
       </c>
@@ -15947,7 +15953,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:25" ht="42" x14ac:dyDescent="0.15">
       <c r="A231" s="8">
         <v>6</v>
       </c>
@@ -16006,7 +16012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="232" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A232" s="8">
         <v>7</v>
       </c>
@@ -16062,7 +16068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A233" s="8">
         <v>7</v>
       </c>
@@ -16121,7 +16127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="234" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A234" s="8">
         <v>7</v>
       </c>
@@ -16180,7 +16186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A235" s="8">
         <v>7</v>
       </c>
@@ -16242,7 +16248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A236" s="8">
         <v>7</v>
       </c>
@@ -16298,7 +16304,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A237" s="8">
         <v>7</v>
       </c>
@@ -16354,7 +16360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A238" s="8">
         <v>7</v>
       </c>
@@ -16416,7 +16422,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A239" s="8">
         <v>7</v>
       </c>
@@ -16472,7 +16478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A240" s="8">
         <v>7</v>
       </c>
@@ -16528,7 +16534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A241" s="8">
         <v>7</v>
       </c>
@@ -16587,7 +16593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A242" s="8">
         <v>7</v>
       </c>
@@ -16643,7 +16649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A243" s="8">
         <v>7</v>
       </c>
@@ -16699,7 +16705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A244" s="8">
         <v>7</v>
       </c>
@@ -16755,7 +16761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A245" s="8">
         <v>7</v>
       </c>
@@ -16802,7 +16808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="246" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A246" s="8">
         <v>7</v>
       </c>
@@ -16864,7 +16870,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A247" s="8">
         <v>7</v>
       </c>
@@ -16920,7 +16926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="248" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A248" s="8">
         <v>7</v>
       </c>
@@ -16976,7 +16982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A249" s="8">
         <v>7</v>
       </c>
@@ -17038,7 +17044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A250" s="8">
         <v>7</v>
       </c>
@@ -17097,7 +17103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="251" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A251" s="8">
         <v>7</v>
       </c>
@@ -17153,7 +17159,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A252" s="8">
         <v>7</v>
       </c>
@@ -17209,7 +17215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A253" s="8">
         <v>7</v>
       </c>
@@ -17259,7 +17265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="254" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A254" s="8">
         <v>7</v>
       </c>
@@ -17315,7 +17321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="255" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A255" s="8">
         <v>7</v>
       </c>
@@ -17371,7 +17377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="256" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A256" s="8">
         <v>7</v>
       </c>
@@ -17427,7 +17433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A257" s="8">
         <v>7</v>
       </c>
@@ -17477,7 +17483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A258" s="8">
         <v>7</v>
       </c>
@@ -17533,7 +17539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A259" s="8">
         <v>7</v>
       </c>
@@ -17589,7 +17595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="260" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A260" s="8">
         <v>7</v>
       </c>
@@ -17645,7 +17651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="261" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A261" s="8">
         <v>7</v>
       </c>
@@ -17701,7 +17707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="262" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A262" s="8">
         <v>7</v>
       </c>
@@ -17757,7 +17763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A263" s="8">
         <v>7</v>
       </c>
@@ -17813,7 +17819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="264" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A264" s="8">
         <v>8</v>
       </c>
@@ -17869,7 +17875,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="265" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A265" s="8">
         <v>8</v>
       </c>
@@ -17928,7 +17934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="266" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A266" s="8">
         <v>8</v>
       </c>
@@ -17987,7 +17993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="267" spans="1:25" ht="57" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:25" ht="56" x14ac:dyDescent="0.15">
       <c r="A267" s="8">
         <v>8</v>
       </c>
@@ -18046,7 +18052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="268" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A268" s="8">
         <v>8</v>
       </c>
@@ -18102,7 +18108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="269" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A269" s="8">
         <v>8</v>
       </c>
@@ -18158,7 +18164,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="270" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A270" s="8">
         <v>8</v>
       </c>
@@ -18217,7 +18223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="271" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A271" s="8">
         <v>8</v>
       </c>
@@ -18276,7 +18282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="272" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A272" s="8">
         <v>8</v>
       </c>
@@ -18332,7 +18338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="273" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A273" s="8">
         <v>8</v>
       </c>
@@ -18391,7 +18397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="274" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A274" s="8">
         <v>8</v>
       </c>
@@ -18447,7 +18453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="275" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A275" s="8">
         <v>8</v>
       </c>
@@ -18503,7 +18509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="276" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A276" s="8">
         <v>8</v>
       </c>
@@ -18562,7 +18568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="277" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A277" s="8">
         <v>8</v>
       </c>
@@ -18621,7 +18627,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="278" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A278" s="8">
         <v>8</v>
       </c>
@@ -18683,7 +18689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="279" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A279" s="8">
         <v>8</v>
       </c>
@@ -18742,7 +18748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="280" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A280" s="8">
         <v>8</v>
       </c>
@@ -18798,7 +18804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="281" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A281" s="8">
         <v>8</v>
       </c>
@@ -18854,7 +18860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="282" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A282" s="8">
         <v>8</v>
       </c>
@@ -18910,7 +18916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="283" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A283" s="8">
         <v>8</v>
       </c>
@@ -18957,7 +18963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A284" s="8">
         <v>8</v>
       </c>
@@ -19013,7 +19019,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="285" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A285" s="8">
         <v>8</v>
       </c>
@@ -19069,7 +19075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="286" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A286" s="8">
         <v>8</v>
       </c>
@@ -19125,7 +19131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="287" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A287" s="8">
         <v>8</v>
       </c>
@@ -19181,7 +19187,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="288" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A288" s="8">
         <v>8</v>
       </c>
@@ -19237,7 +19243,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="289" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A289" s="8">
         <v>8</v>
       </c>
@@ -19293,7 +19299,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A290" s="8">
         <v>8</v>
       </c>
@@ -19349,7 +19355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A291" s="8">
         <v>8</v>
       </c>
@@ -19408,7 +19414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A292" s="8">
         <v>8</v>
       </c>
@@ -19464,7 +19470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A293" s="8">
         <v>8</v>
       </c>
@@ -19523,7 +19529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="294" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A294" s="8">
         <v>8</v>
       </c>
@@ -19579,7 +19585,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="295" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A295" s="8">
         <v>8</v>
       </c>
@@ -19635,7 +19641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A296" s="8">
         <v>8</v>
       </c>
@@ -19691,7 +19697,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="297" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A297" s="8">
         <v>8</v>
       </c>
@@ -19747,7 +19753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="298" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A298" s="8">
         <v>8</v>
       </c>
@@ -19803,7 +19809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A299" s="8">
         <v>8</v>
       </c>
@@ -19859,7 +19865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="300" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A300" s="8">
         <v>8</v>
       </c>
@@ -19915,7 +19921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="301" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A301" s="8">
         <v>8</v>
       </c>
@@ -19971,7 +19977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="302" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A302" s="8">
         <v>8</v>
       </c>
@@ -20027,7 +20033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="303" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A303" s="8">
         <v>8</v>
       </c>
@@ -20083,7 +20089,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="304" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A304" s="8">
         <v>8</v>
       </c>
@@ -20139,7 +20145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="305" spans="1:25" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:25" ht="28" x14ac:dyDescent="0.15">
       <c r="A305" s="8">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
adds more cols to script
</commit_message>
<xml_diff>
--- a/film charting stafford 2016.xlsx
+++ b/film charting stafford 2016.xlsx
@@ -151,7 +151,7 @@
     <definedName name="pbp_97" localSheetId="0">'Drive Chart'!#REF!</definedName>
     <definedName name="pbp_99" localSheetId="0">'Drive Chart'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -167,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3990" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3989" uniqueCount="647">
   <si>
     <t>Pass Area</t>
   </si>
@@ -2652,9 +2652,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ305"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J306" sqref="J306"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q98" sqref="Q98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -8466,10 +8466,10 @@
         <v>553</v>
       </c>
       <c r="P97" s="8" t="s">
-        <v>317</v>
-      </c>
-      <c r="Q97" s="8" t="s">
         <v>559</v>
+      </c>
+      <c r="Q97" s="8">
+        <v>0</v>
       </c>
       <c r="T97" s="8" t="s">
         <v>439</v>

</xml_diff>